<commit_message>
Añadido de formatos y regex de validacion, arreglo fallos
</commit_message>
<xml_diff>
--- a/AI_Engine/Resultados/99999TSE01/dataFrame.xlsx
+++ b/AI_Engine/Resultados/99999TSE01/dataFrame.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,67 +481,1398 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t78.pdf</t>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t101.pdf</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4501157689</t>
+          <t>4501163359</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>JD REMAN</t>
+          <t>99999TSE01</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>RE56369</t>
+          <t>R104589</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>490</t>
+          <t>200</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>08/27/2021</t>
+          <t>11/16/2021</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
-        <v>90.155</v>
+        <v>90.02500000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t78.pdf</t>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t107.pdf</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4501157689</t>
+          <t>4501162345</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>JD REMAN</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>R71037</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>08/27/2021</t>
+          <t>10/15/2021</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
+        <v>85.098</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t107.pdf</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>4501162345</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>10/15/2021</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t108.pdf</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4501159414</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>R518255</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>188</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>08/19/2021</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>75.82299999999999</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t108.pdf</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>4501159414</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>08/19/2021</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t117.pdf</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>4501161062</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>R528098</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>08/31/2021</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>86.22499999999999</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t117.pdf</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>4501161062</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>08/31/2021</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t119.pdf</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>4501158323</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>RE500631</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>310</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>09/27/2021</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>89.61799999999999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t119.pdf</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>4501158323</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>09/27/2021</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t125.pdf</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>4501157689</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>RE56369</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>490</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>08/27/2021</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>72.67400000000001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t125.pdf</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4501157689</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>08/27/2021</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t127.pdf</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>4501160257</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>R528098</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>08/25/2021</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>86.22499999999999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t127.pdf</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>4501160257</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>08/25/2021</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t128.pdf</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4501159414</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>R518255</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>188</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>08/19/2021</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>75.82299999999999</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t128.pdf</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>4501159414</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>08/19/2021</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t50.pdf</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>4501169494</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>S250</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>160</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>12/02/2021</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="n">
+        <v>69.054</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t52.pdf</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>4501169440</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>R516237</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>432</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>09/28/2021</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>69.054</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t53.pdf</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>4501169439</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>R529655</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>11/30/2021</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="n">
+        <v>69.054</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t62.pdf</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>4501169494</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>S250</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>160</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>12/02/2021</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="n">
+        <v>69.054</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t64.pdf</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>4501169440</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>R516237</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>432</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>09/28/2021</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="n">
+        <v>69.054</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t65.pdf</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>4501169439</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>R529655</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>11/30/2021</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>69.054</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t73.pdf</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>4501165400</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>RE508489</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>224</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>10/25/2021</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="n">
+        <v>69.054</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t74.pdf</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>4501165399</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>R71037</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>10/27/2021</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>85.098</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t74.pdf</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>4501165399</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>10/27/2021</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t76.pdf</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>4501165398</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>R528098</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>10/06/2021</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="n">
+        <v>86.22499999999999</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t76.pdf</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>4501165398</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>10/06/2021</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t78.pdf</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>4501157689</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>RE56369</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>490</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>08/27/2021</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="n">
+        <v>72.67400000000001</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t78.pdf</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>4501157689</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>08/27/2021</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t83.pdf</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>4501163359</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>R104589</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>11/16/2021</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="n">
+        <v>90.02500000000001</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t83.pdf</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>4501163359</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>11/16/2021</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t89.pdf</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>4501165400</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>RE508489</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>224</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>10/25/2021</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="n">
+        <v>69.054</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t90.pdf</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>4501165399</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>R71037</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>10/27/2021</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="n">
+        <v>85.098</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t90.pdf</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>4501165399</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>10/27/2021</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t92.pdf</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>4501165398</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>R528098</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>10/06/2021</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="n">
+        <v>86.22499999999999</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t92.pdf</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>4501165398</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>10/06/2021</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t94.pdf</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>4501157689</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>RE56369</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>490</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>08/27/2021</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="n">
+        <v>72.67400000000001</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t94.pdf</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>4501157689</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>08/27/2021</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t99.pdf</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>4501161062</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>R528098</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>08/31/2021</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="n">
+        <v>86.22499999999999</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\JD REMAN\t99.pdf</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>4501161062</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>99999TSE01</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>08/31/2021</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="n">
         <v>-100</v>
       </c>
     </row>

</xml_diff>